<commit_message>
2012-9-13 sashimi  configure the ip address.
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/keywordscripts/TST425_SetActionForAlarmOrEvent.xlsx
+++ b/NformTester/NformTester/keywordscripts/TST425_SetActionForAlarmOrEvent.xlsx
@@ -1208,7 +1208,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7603" uniqueCount="846">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7603" uniqueCount="845">
   <si>
     <t>FormLogin_to_LiebertR_Nform</t>
   </si>
@@ -3661,9 +3661,6 @@
     <t>SingleManual</t>
   </si>
   <si>
-    <t>"ABC GXT UPS"</t>
-  </si>
-  <si>
     <t>"Description for GXT"</t>
   </si>
   <si>
@@ -3671,10 +3668,6 @@
   </si>
   <si>
     <t>"SNMP"</t>
-  </si>
-  <si>
-    <t>10.146.83.10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Pause</t>
@@ -3778,10 +3771,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ABC GXT UPS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>;Create an action, add three actions, Run-command,Email and write file.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3796,6 +3785,12 @@
   <si>
     <t xml:space="preserve">;Prerequisites 1. NformG2 software installed on windows operating System. 2. Advanced communication license must be added before adding devices. 3. User should have permission to 'Write Data Action' under Groups. 4. SNMP devices should be added before going for test action. </t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$SNMPdevice_0$</t>
+  </si>
+  <si>
+    <t>$GXT_0$</t>
   </si>
 </sst>
 </file>
@@ -4781,8 +4776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="F77" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H109" sqref="H109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4945,7 +4940,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -4970,7 +4965,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -5014,7 +5009,7 @@
         <v>765</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C8" s="5">
         <v>7</v>
@@ -5033,19 +5028,19 @@
         <v>806</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>811</v>
+        <v>843</v>
       </c>
       <c r="J8" s="5" t="s">
+        <v>844</v>
+      </c>
+      <c r="K8" s="5" t="s">
         <v>807</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="L8" s="5" t="s">
         <v>808</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="M8" s="5" t="s">
         <v>809</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>810</v>
       </c>
       <c r="N8" s="7"/>
       <c r="O8" s="2"/>
@@ -5061,7 +5056,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="5"/>
@@ -5082,7 +5077,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>19</v>
@@ -5111,7 +5106,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>19</v>
@@ -5140,7 +5135,7 @@
         <v>11</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>306</v>
@@ -5152,7 +5147,7 @@
         <v>7</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="I12" s="5" t="b">
         <v>1</v>
@@ -5200,7 +5195,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>306</v>
@@ -5229,7 +5224,7 @@
         <v>14</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>310</v>
@@ -5241,7 +5236,7 @@
         <v>4</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -5260,7 +5255,7 @@
         <v>15</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>310</v>
@@ -5272,7 +5267,7 @@
         <v>4</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
@@ -5291,7 +5286,7 @@
         <v>16</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>310</v>
@@ -5380,7 +5375,7 @@
         <v>19</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>317</v>
@@ -5392,7 +5387,7 @@
         <v>4</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="I20" s="11"/>
       <c r="J20" s="5"/>
@@ -5411,7 +5406,7 @@
         <v>20</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="E21" s="11" t="s">
         <v>317</v>
@@ -5423,7 +5418,7 @@
         <v>4</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="I21" s="11"/>
       <c r="J21" s="5"/>
@@ -5450,7 +5445,7 @@
         <v>13</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>841</v>
+        <v>844</v>
       </c>
       <c r="I22" s="11"/>
       <c r="J22" s="5"/>
@@ -5494,7 +5489,7 @@
         <v>23</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>317</v>
@@ -5585,7 +5580,7 @@
         <v>4</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="I27" s="11"/>
       <c r="J27" s="5"/>
@@ -5637,7 +5632,7 @@
         <v>59</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="I29" s="11"/>
       <c r="J29" s="5"/>
@@ -5762,7 +5757,7 @@
         <v>4</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="I34" s="11"/>
       <c r="J34" s="5"/>
@@ -5789,7 +5784,7 @@
         <v>4</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="I35" s="11"/>
       <c r="J35" s="5"/>
@@ -5816,7 +5811,7 @@
         <v>4</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="I36" s="11"/>
       <c r="J36" s="5"/>
@@ -5843,7 +5838,7 @@
         <v>4</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="I37" s="11"/>
       <c r="J37" s="5"/>
@@ -5870,7 +5865,7 @@
         <v>4</v>
       </c>
       <c r="H38" s="11" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="I38" s="11"/>
       <c r="J38" s="5"/>
@@ -6043,7 +6038,7 @@
         <v>4</v>
       </c>
       <c r="H45" s="11" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
@@ -6070,7 +6065,7 @@
         <v>4</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
@@ -6176,7 +6171,7 @@
         <v>4</v>
       </c>
       <c r="H50" s="18" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
@@ -6228,7 +6223,7 @@
         <v>4</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
@@ -6255,7 +6250,7 @@
         <v>4</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
@@ -6282,7 +6277,7 @@
         <v>4</v>
       </c>
       <c r="H54" s="11" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="I54" s="11"/>
       <c r="J54" s="5"/>
@@ -6384,7 +6379,7 @@
         <v>13</v>
       </c>
       <c r="H58" s="11" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="I58" s="11"/>
       <c r="J58" s="5"/>
@@ -6411,7 +6406,7 @@
         <v>13</v>
       </c>
       <c r="H59" s="11" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="I59" s="11"/>
       <c r="J59" s="5"/>
@@ -6549,7 +6544,7 @@
         <v>76</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="E65" s="11" t="s">
         <v>306</v>
@@ -6586,7 +6581,7 @@
         <v>59</v>
       </c>
       <c r="H66" s="11" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="I66" s="5"/>
       <c r="J66" s="5"/>
@@ -6674,7 +6669,7 @@
         <v>81</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="E70" s="11"/>
       <c r="F70" s="5"/>
@@ -6755,7 +6750,7 @@
         <v>56</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>807</v>
+        <v>844</v>
       </c>
       <c r="I73" s="5"/>
       <c r="J73" s="5"/>
@@ -6935,10 +6930,10 @@
         <v>115</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="F81" s="5">
         <v>2</v>
@@ -6966,7 +6961,7 @@
         <v>22</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
@@ -6991,7 +6986,7 @@
         <v>83</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="H83" s="5"/>
       <c r="I83" s="5"/>
@@ -7016,7 +7011,7 @@
         <v>401</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="H84" s="5"/>
       <c r="I84" s="5"/>
@@ -7072,7 +7067,7 @@
         <v>358</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="H86" s="5"/>
       <c r="I86" s="5"/>
@@ -7218,7 +7213,7 @@
         <v>7</v>
       </c>
       <c r="H91" s="5" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="I91" s="5" t="b">
         <v>1</v>
@@ -7247,7 +7242,7 @@
         <v>7</v>
       </c>
       <c r="H92" s="5" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="I92" s="5" t="s">
         <v>798</v>
@@ -7303,7 +7298,7 @@
         <v>7</v>
       </c>
       <c r="H94" s="5" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="I94" s="5" t="s">
         <v>798</v>
@@ -7359,13 +7354,13 @@
         <v>7</v>
       </c>
       <c r="H96" s="5" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="I96" s="5" t="s">
         <v>798</v>
       </c>
       <c r="J96" s="5" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="K96" s="5"/>
       <c r="L96" s="5"/>
@@ -7390,13 +7385,13 @@
         <v>7</v>
       </c>
       <c r="H97" s="5" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="I97" s="5" t="s">
         <v>798</v>
       </c>
       <c r="J97" s="5" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="K97" s="5"/>
       <c r="L97" s="5"/>
@@ -7421,7 +7416,7 @@
         <v>4</v>
       </c>
       <c r="H98" s="5" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="I98" s="5"/>
       <c r="J98" s="5"/>
@@ -7448,7 +7443,7 @@
         <v>4</v>
       </c>
       <c r="H99" s="5" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="I99" s="5"/>
       <c r="J99" s="5"/>
@@ -7536,10 +7531,10 @@
         <v>137</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="E103" s="11" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="F103" s="5" t="s">
         <v>578</v>
@@ -7548,7 +7543,7 @@
         <v>3</v>
       </c>
       <c r="H103" s="5" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="I103" s="5"/>
       <c r="J103" s="5"/>
@@ -7562,10 +7557,10 @@
         <v>138</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="E104" s="11" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="F104" s="5" t="s">
         <v>184</v>
@@ -7586,7 +7581,7 @@
         <v>139</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="E105" s="5" t="s">
         <v>585</v>
@@ -7610,10 +7605,10 @@
         <v>140</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="E106" s="11" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="F106" s="5" t="s">
         <v>99</v>

</xml_diff>

<commit_message>
Unity the node name in Device.ini
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/keywordscripts/TST425_SetActionForAlarmOrEvent.xlsx
+++ b/NformTester/NformTester/keywordscripts/TST425_SetActionForAlarmOrEvent.xlsx
@@ -1208,7 +1208,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7603" uniqueCount="845">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7604" uniqueCount="846">
   <si>
     <t>FormLogin_to_LiebertR_Nform</t>
   </si>
@@ -3791,6 +3791,10 @@
   </si>
   <si>
     <t>$GXT_0$</t>
+  </si>
+  <si>
+    <t>Running Range</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -4776,8 +4780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F77" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H109" sqref="H109"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -5006,11 +5010,9 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="3" t="s">
-        <v>765</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>821</v>
-      </c>
+        <v>845</v>
+      </c>
+      <c r="B8" s="4"/>
       <c r="C8" s="5">
         <v>7</v>
       </c>
@@ -5047,10 +5049,10 @@
     </row>
     <row r="9" spans="1:15" ht="15">
       <c r="A9" s="3" t="s">
-        <v>775</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>776</v>
+        <v>765</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>821</v>
       </c>
       <c r="C9" s="5">
         <v>8</v>
@@ -5071,8 +5073,12 @@
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14"/>
+      <c r="A10" s="3" t="s">
+        <v>775</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>776</v>
+      </c>
       <c r="C10" s="5">
         <v>9</v>
       </c>
@@ -5098,10 +5104,8 @@
       <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="3" t="s">
-        <v>777</v>
-      </c>
-      <c r="B11" s="15"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="5">
         <v>10</v>
       </c>
@@ -5128,7 +5132,7 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="3" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="5">
@@ -5161,7 +5165,7 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="3" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="5">
@@ -5188,7 +5192,7 @@
     </row>
     <row r="14" spans="1:15">
       <c r="A14" s="3" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="5">
@@ -5217,7 +5221,7 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="3" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="5">
@@ -5248,7 +5252,7 @@
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="3" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="5">
@@ -5278,10 +5282,10 @@
       <c r="O16" s="2"/>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="3"/>
-      <c r="B17" s="15" t="s">
-        <v>783</v>
-      </c>
+      <c r="A17" s="3" t="s">
+        <v>782</v>
+      </c>
+      <c r="B17" s="15"/>
       <c r="C17" s="5">
         <v>16</v>
       </c>
@@ -5309,7 +5313,7 @@
     <row r="18" spans="1:15">
       <c r="A18" s="3"/>
       <c r="B18" s="15" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="C18" s="5">
         <v>17</v>
@@ -5336,11 +5340,9 @@
       <c r="O18" s="2"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="3" t="s">
-        <v>785</v>
-      </c>
+      <c r="A19" s="3"/>
       <c r="B19" s="15" t="s">
-        <v>776</v>
+        <v>784</v>
       </c>
       <c r="C19" s="5">
         <v>18</v>
@@ -5368,9 +5370,11 @@
     </row>
     <row r="20" spans="1:15">
       <c r="A20" s="3" t="s">
-        <v>786</v>
-      </c>
-      <c r="B20" s="15"/>
+        <v>785</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>776</v>
+      </c>
       <c r="C20" s="5">
         <v>19</v>
       </c>
@@ -5399,7 +5403,7 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="3" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="5">
@@ -5429,6 +5433,10 @@
       <c r="O21" s="2"/>
     </row>
     <row r="22" spans="1:15">
+      <c r="A22" s="3" t="s">
+        <v>787</v>
+      </c>
+      <c r="B22" s="15"/>
       <c r="C22" s="5">
         <v>21</v>
       </c>
@@ -6802,6 +6810,7 @@
       <c r="L75" s="5"/>
       <c r="M75" s="5"/>
       <c r="N75" s="7"/>
+      <c r="O75" s="2"/>
     </row>
     <row r="76" spans="3:15">
       <c r="C76" s="5">
@@ -6970,7 +6979,6 @@
       <c r="L82" s="5"/>
       <c r="M82" s="5"/>
       <c r="N82" s="7"/>
-      <c r="O82" s="2"/>
     </row>
     <row r="83" spans="3:15">
       <c r="C83" s="5">
@@ -7501,6 +7509,7 @@
       <c r="L101" s="5"/>
       <c r="M101" s="5"/>
       <c r="N101" s="16"/>
+      <c r="O101" s="2"/>
     </row>
     <row r="102" spans="3:15">
       <c r="C102" s="5">
@@ -7651,7 +7660,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D76:D81 D101:D102 D43:D69 D33 D10:D26 D3:D4 D8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D76:D81 D101:D102 D43:D69 D33 D10:D26 D8 D3:D4">
       <formula1>"C,F,T,;"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G104:G106 G2:G102">

</xml_diff>